<commit_message>
- Update data sets - adding multilevel models incl. random slopes
</commit_message>
<xml_diff>
--- a/Data_EE Downward Causation_Conjoint_Wave5.xlsx
+++ b/Data_EE Downward Causation_Conjoint_Wave5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johannes.haehnlein\Desktop\Johannes Haehnlein\19_PROMOTION\01_STUDIEN\Studie 2 - Conjoint\Data\R Repository\EE_Downward-Causation_Entrepreneurship-Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9671D4D-71C9-48B0-A1F0-F49A2EE8ED6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C1709C-C5C5-4F9F-8524-61637835A780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studie zur Stärkung von Gründun" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="146">
   <si>
     <t>age</t>
   </si>
@@ -466,6 +466,12 @@
   <si>
     <t>Neumarkt</t>
   </si>
+  <si>
+    <t>Aschaffenburg</t>
+  </si>
+  <si>
+    <t>Wietzendorf</t>
+  </si>
 </sst>
 </file>
 
@@ -818,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BZ130"/>
+  <dimension ref="A1:BZ134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128"/>
+    <sheetView tabSelected="1" topLeftCell="S100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z141" sqref="Z141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -831,7 +837,7 @@
     <col min="17" max="18" width="11.44140625"/>
     <col min="19" max="19" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="26" width="11.44140625"/>
-    <col min="27" max="27" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="28" max="35" width="11.44140625"/>
     <col min="36" max="36" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="37" max="40" width="11.44140625"/>
@@ -31476,6 +31482,947 @@
         <v>10.258999999999999</v>
       </c>
     </row>
+    <row r="131" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>25</v>
+      </c>
+      <c r="B131" s="2">
+        <v>1</v>
+      </c>
+      <c r="C131" s="2">
+        <v>6</v>
+      </c>
+      <c r="D131" s="2">
+        <v>6</v>
+      </c>
+      <c r="E131" s="2">
+        <v>1</v>
+      </c>
+      <c r="F131" s="2">
+        <v>1</v>
+      </c>
+      <c r="G131" s="2">
+        <v>2</v>
+      </c>
+      <c r="H131" s="2">
+        <v>0</v>
+      </c>
+      <c r="J131" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K131" s="2">
+        <v>0</v>
+      </c>
+      <c r="L131" s="2">
+        <v>0</v>
+      </c>
+      <c r="M131" s="2">
+        <v>0</v>
+      </c>
+      <c r="N131" s="2">
+        <v>0</v>
+      </c>
+      <c r="O131" s="2">
+        <v>6</v>
+      </c>
+      <c r="P131" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q131" s="2">
+        <v>3</v>
+      </c>
+      <c r="R131" s="2">
+        <v>4</v>
+      </c>
+      <c r="S131" s="2">
+        <v>6</v>
+      </c>
+      <c r="T131" s="2">
+        <v>3</v>
+      </c>
+      <c r="U131" s="2">
+        <v>4</v>
+      </c>
+      <c r="V131" s="2">
+        <v>5</v>
+      </c>
+      <c r="W131" s="2">
+        <v>7</v>
+      </c>
+      <c r="X131" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y131" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z131" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA131" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AC131" s="2">
+        <v>4</v>
+      </c>
+      <c r="AD131" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE131" s="2">
+        <v>4</v>
+      </c>
+      <c r="AF131" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG131" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AJ131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AK131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AL131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AM131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AN131" s="2">
+        <v>7</v>
+      </c>
+      <c r="AO131" s="2">
+        <v>7</v>
+      </c>
+      <c r="AP131" s="2">
+        <v>7</v>
+      </c>
+      <c r="AQ131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AR131" s="2">
+        <v>5</v>
+      </c>
+      <c r="AS131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AT131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AU131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AV131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AW131" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX131" s="2">
+        <v>6</v>
+      </c>
+      <c r="AY131" s="2">
+        <v>5</v>
+      </c>
+      <c r="AZ131" s="2">
+        <v>7</v>
+      </c>
+      <c r="BA131" s="2">
+        <v>5</v>
+      </c>
+      <c r="BB131" s="2">
+        <v>6</v>
+      </c>
+      <c r="BC131" s="2">
+        <v>5</v>
+      </c>
+      <c r="BD131" s="2">
+        <v>5</v>
+      </c>
+      <c r="BE131" s="2">
+        <v>3</v>
+      </c>
+      <c r="BF131" s="2">
+        <v>5</v>
+      </c>
+      <c r="BG131" s="2">
+        <v>5</v>
+      </c>
+      <c r="BH131" s="2">
+        <v>6</v>
+      </c>
+      <c r="BI131" s="2">
+        <v>6</v>
+      </c>
+      <c r="BJ131" s="2">
+        <v>3</v>
+      </c>
+      <c r="BK131" s="2">
+        <v>5</v>
+      </c>
+      <c r="BL131" s="2">
+        <v>1</v>
+      </c>
+      <c r="BM131" s="2">
+        <v>3</v>
+      </c>
+      <c r="BN131" s="2">
+        <v>5</v>
+      </c>
+      <c r="BO131" s="2">
+        <v>5</v>
+      </c>
+      <c r="BP131" s="2">
+        <v>4</v>
+      </c>
+      <c r="BQ131" s="2">
+        <v>7</v>
+      </c>
+      <c r="BR131" s="2">
+        <v>7</v>
+      </c>
+      <c r="BS131" s="2">
+        <v>7</v>
+      </c>
+      <c r="BT131" s="2">
+        <v>4</v>
+      </c>
+      <c r="BU131" s="2">
+        <v>4</v>
+      </c>
+      <c r="BV131" s="2">
+        <v>4</v>
+      </c>
+      <c r="BW131" s="2">
+        <v>4</v>
+      </c>
+      <c r="BX131" s="2">
+        <v>4</v>
+      </c>
+      <c r="BY131" s="2">
+        <v>4</v>
+      </c>
+      <c r="BZ131" s="3">
+        <v>17.438666666666666</v>
+      </c>
+    </row>
+    <row r="132" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>33</v>
+      </c>
+      <c r="B132" s="2">
+        <v>2</v>
+      </c>
+      <c r="C132" s="2">
+        <v>6</v>
+      </c>
+      <c r="D132" s="2">
+        <v>5</v>
+      </c>
+      <c r="E132" s="2">
+        <v>1</v>
+      </c>
+      <c r="F132" s="2">
+        <v>1</v>
+      </c>
+      <c r="G132" s="2">
+        <v>4</v>
+      </c>
+      <c r="H132" s="2">
+        <v>1</v>
+      </c>
+      <c r="I132" s="2">
+        <v>6</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K132" s="2">
+        <v>2</v>
+      </c>
+      <c r="L132" s="2">
+        <v>0</v>
+      </c>
+      <c r="M132" s="2">
+        <v>0</v>
+      </c>
+      <c r="N132" s="2">
+        <v>0</v>
+      </c>
+      <c r="O132" s="2">
+        <v>6</v>
+      </c>
+      <c r="P132" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q132" s="2">
+        <v>5</v>
+      </c>
+      <c r="R132" s="2">
+        <v>4</v>
+      </c>
+      <c r="S132" s="2">
+        <v>6</v>
+      </c>
+      <c r="T132" s="2">
+        <v>5</v>
+      </c>
+      <c r="U132" s="2">
+        <v>5</v>
+      </c>
+      <c r="V132" s="2">
+        <v>6</v>
+      </c>
+      <c r="W132" s="2">
+        <v>7</v>
+      </c>
+      <c r="X132" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y132" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z132" s="2">
+        <v>6</v>
+      </c>
+      <c r="AA132" s="2">
+        <v>4</v>
+      </c>
+      <c r="AB132" s="2">
+        <v>6</v>
+      </c>
+      <c r="AC132" s="2">
+        <v>5</v>
+      </c>
+      <c r="AD132" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE132" s="2">
+        <v>6</v>
+      </c>
+      <c r="AF132" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG132" s="2">
+        <v>6</v>
+      </c>
+      <c r="AH132" s="2">
+        <v>5</v>
+      </c>
+      <c r="AI132" s="2">
+        <v>6</v>
+      </c>
+      <c r="AJ132" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK132" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL132" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM132" s="2">
+        <v>5</v>
+      </c>
+      <c r="AN132" s="2">
+        <v>6</v>
+      </c>
+      <c r="AO132" s="2">
+        <v>5</v>
+      </c>
+      <c r="AP132" s="2">
+        <v>5</v>
+      </c>
+      <c r="AQ132" s="2">
+        <v>5</v>
+      </c>
+      <c r="AR132" s="2">
+        <v>6</v>
+      </c>
+      <c r="AS132" s="2">
+        <v>5</v>
+      </c>
+      <c r="AT132" s="2">
+        <v>6</v>
+      </c>
+      <c r="AU132" s="2">
+        <v>6</v>
+      </c>
+      <c r="AV132" s="2">
+        <v>6</v>
+      </c>
+      <c r="AW132" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX132" s="2">
+        <v>2</v>
+      </c>
+      <c r="AY132" s="2">
+        <v>3</v>
+      </c>
+      <c r="AZ132" s="2">
+        <v>5</v>
+      </c>
+      <c r="BA132" s="2">
+        <v>3</v>
+      </c>
+      <c r="BB132" s="2">
+        <v>4</v>
+      </c>
+      <c r="BC132" s="2">
+        <v>5</v>
+      </c>
+      <c r="BD132" s="2">
+        <v>4</v>
+      </c>
+      <c r="BE132" s="2">
+        <v>2</v>
+      </c>
+      <c r="BF132" s="2">
+        <v>5</v>
+      </c>
+      <c r="BG132" s="2">
+        <v>3</v>
+      </c>
+      <c r="BH132" s="2">
+        <v>3</v>
+      </c>
+      <c r="BI132" s="2">
+        <v>1</v>
+      </c>
+      <c r="BJ132" s="2">
+        <v>5</v>
+      </c>
+      <c r="BK132" s="2">
+        <v>4</v>
+      </c>
+      <c r="BL132" s="2">
+        <v>1</v>
+      </c>
+      <c r="BM132" s="2">
+        <v>2</v>
+      </c>
+      <c r="BN132" s="2">
+        <v>5</v>
+      </c>
+      <c r="BO132" s="2">
+        <v>5</v>
+      </c>
+      <c r="BP132" s="2">
+        <v>5</v>
+      </c>
+      <c r="BQ132" s="2">
+        <v>6</v>
+      </c>
+      <c r="BR132" s="2">
+        <v>6</v>
+      </c>
+      <c r="BS132" s="2">
+        <v>6</v>
+      </c>
+      <c r="BT132" s="2">
+        <v>2</v>
+      </c>
+      <c r="BU132" s="2">
+        <v>2</v>
+      </c>
+      <c r="BV132" s="2">
+        <v>3</v>
+      </c>
+      <c r="BW132" s="2">
+        <v>2</v>
+      </c>
+      <c r="BX132" s="2">
+        <v>4</v>
+      </c>
+      <c r="BY132" s="2">
+        <v>2</v>
+      </c>
+      <c r="BZ132" s="3">
+        <v>18.89</v>
+      </c>
+    </row>
+    <row r="133" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>35</v>
+      </c>
+      <c r="B133" s="2">
+        <v>2</v>
+      </c>
+      <c r="C133" s="2">
+        <v>6</v>
+      </c>
+      <c r="D133" s="2">
+        <v>5</v>
+      </c>
+      <c r="E133" s="2">
+        <v>1</v>
+      </c>
+      <c r="F133" s="2">
+        <v>1</v>
+      </c>
+      <c r="G133" s="2">
+        <v>2</v>
+      </c>
+      <c r="H133" s="2">
+        <v>1</v>
+      </c>
+      <c r="I133" s="2">
+        <v>5</v>
+      </c>
+      <c r="J133" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K133" s="2">
+        <v>1</v>
+      </c>
+      <c r="L133" s="2">
+        <v>1</v>
+      </c>
+      <c r="M133" s="2">
+        <v>1</v>
+      </c>
+      <c r="N133" s="2">
+        <v>0</v>
+      </c>
+      <c r="O133" s="2">
+        <v>6</v>
+      </c>
+      <c r="P133" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q133" s="2">
+        <v>4</v>
+      </c>
+      <c r="R133" s="2">
+        <v>6</v>
+      </c>
+      <c r="S133" s="2">
+        <v>7</v>
+      </c>
+      <c r="T133" s="2">
+        <v>3</v>
+      </c>
+      <c r="U133" s="2">
+        <v>5</v>
+      </c>
+      <c r="V133" s="2">
+        <v>6</v>
+      </c>
+      <c r="W133" s="2">
+        <v>7</v>
+      </c>
+      <c r="X133" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y133" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z133" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AB133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AC133" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD133" s="2">
+        <v>5</v>
+      </c>
+      <c r="AE133" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF133" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG133" s="2">
+        <v>4</v>
+      </c>
+      <c r="AH133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI133" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ133" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AL133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AM133" s="2">
+        <v>7</v>
+      </c>
+      <c r="AN133" s="2">
+        <v>7</v>
+      </c>
+      <c r="AO133" s="2">
+        <v>5</v>
+      </c>
+      <c r="AP133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AQ133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AR133" s="2">
+        <v>4</v>
+      </c>
+      <c r="AS133" s="2">
+        <v>7</v>
+      </c>
+      <c r="AT133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AU133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AV133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AW133" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX133" s="2">
+        <v>6</v>
+      </c>
+      <c r="AY133" s="2">
+        <v>5</v>
+      </c>
+      <c r="AZ133" s="2">
+        <v>7</v>
+      </c>
+      <c r="BA133" s="2">
+        <v>4</v>
+      </c>
+      <c r="BB133" s="2">
+        <v>6</v>
+      </c>
+      <c r="BC133" s="2">
+        <v>6</v>
+      </c>
+      <c r="BD133" s="2">
+        <v>5</v>
+      </c>
+      <c r="BE133" s="2">
+        <v>3</v>
+      </c>
+      <c r="BF133" s="2">
+        <v>4</v>
+      </c>
+      <c r="BG133" s="2">
+        <v>2</v>
+      </c>
+      <c r="BH133" s="2">
+        <v>5</v>
+      </c>
+      <c r="BI133" s="2">
+        <v>4</v>
+      </c>
+      <c r="BJ133" s="2">
+        <v>3</v>
+      </c>
+      <c r="BK133" s="2">
+        <v>5</v>
+      </c>
+      <c r="BL133" s="2">
+        <v>2</v>
+      </c>
+      <c r="BM133" s="2">
+        <v>1</v>
+      </c>
+      <c r="BN133" s="2">
+        <v>3</v>
+      </c>
+      <c r="BO133" s="2">
+        <v>6</v>
+      </c>
+      <c r="BP133" s="2">
+        <v>6</v>
+      </c>
+      <c r="BQ133" s="2">
+        <v>6</v>
+      </c>
+      <c r="BR133" s="2">
+        <v>6</v>
+      </c>
+      <c r="BS133" s="2">
+        <v>6</v>
+      </c>
+      <c r="BT133" s="2">
+        <v>3</v>
+      </c>
+      <c r="BU133" s="2">
+        <v>3</v>
+      </c>
+      <c r="BV133" s="2">
+        <v>4</v>
+      </c>
+      <c r="BW133" s="2">
+        <v>3</v>
+      </c>
+      <c r="BX133" s="2">
+        <v>4</v>
+      </c>
+      <c r="BY133" s="2">
+        <v>5</v>
+      </c>
+      <c r="BZ133" s="3">
+        <v>32.15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>37</v>
+      </c>
+      <c r="B134" s="2">
+        <v>2</v>
+      </c>
+      <c r="C134" s="2">
+        <v>6</v>
+      </c>
+      <c r="D134" s="2">
+        <v>10</v>
+      </c>
+      <c r="E134" s="2">
+        <v>1</v>
+      </c>
+      <c r="F134" s="2">
+        <v>3</v>
+      </c>
+      <c r="G134" s="2">
+        <v>8</v>
+      </c>
+      <c r="H134" s="2">
+        <v>1</v>
+      </c>
+      <c r="I134" s="2">
+        <v>1</v>
+      </c>
+      <c r="J134" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K134" s="2">
+        <v>7</v>
+      </c>
+      <c r="L134" s="2">
+        <v>1</v>
+      </c>
+      <c r="M134" s="2">
+        <v>1</v>
+      </c>
+      <c r="N134" s="2">
+        <v>0</v>
+      </c>
+      <c r="O134" s="2">
+        <v>6</v>
+      </c>
+      <c r="P134" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q134" s="2">
+        <v>3</v>
+      </c>
+      <c r="R134" s="2">
+        <v>4</v>
+      </c>
+      <c r="S134" s="2">
+        <v>6</v>
+      </c>
+      <c r="T134" s="2">
+        <v>3</v>
+      </c>
+      <c r="U134" s="2">
+        <v>4</v>
+      </c>
+      <c r="V134" s="2">
+        <v>4</v>
+      </c>
+      <c r="W134" s="2">
+        <v>6</v>
+      </c>
+      <c r="X134" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y134" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z134" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA134" s="2">
+        <v>4</v>
+      </c>
+      <c r="AB134" s="2">
+        <v>5</v>
+      </c>
+      <c r="AC134" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD134" s="2">
+        <v>4</v>
+      </c>
+      <c r="AE134" s="2">
+        <v>4</v>
+      </c>
+      <c r="AF134" s="2">
+        <v>6</v>
+      </c>
+      <c r="AG134" s="2">
+        <v>5</v>
+      </c>
+      <c r="AH134" s="2">
+        <v>2</v>
+      </c>
+      <c r="AI134" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ134" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK134" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL134" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM134" s="2">
+        <v>5</v>
+      </c>
+      <c r="AN134" s="2">
+        <v>6</v>
+      </c>
+      <c r="AO134" s="2">
+        <v>7</v>
+      </c>
+      <c r="AP134" s="2">
+        <v>6</v>
+      </c>
+      <c r="AQ134" s="2">
+        <v>4</v>
+      </c>
+      <c r="AR134" s="2">
+        <v>6</v>
+      </c>
+      <c r="AS134" s="2">
+        <v>7</v>
+      </c>
+      <c r="AT134" s="2">
+        <v>7</v>
+      </c>
+      <c r="AU134" s="2">
+        <v>7</v>
+      </c>
+      <c r="AV134" s="2">
+        <v>6</v>
+      </c>
+      <c r="AW134" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX134" s="2">
+        <v>5</v>
+      </c>
+      <c r="AY134" s="2">
+        <v>5</v>
+      </c>
+      <c r="AZ134" s="2">
+        <v>5</v>
+      </c>
+      <c r="BA134" s="2">
+        <v>6</v>
+      </c>
+      <c r="BB134" s="2">
+        <v>5</v>
+      </c>
+      <c r="BC134" s="2">
+        <v>4</v>
+      </c>
+      <c r="BD134" s="2">
+        <v>4</v>
+      </c>
+      <c r="BE134" s="2">
+        <v>4</v>
+      </c>
+      <c r="BF134" s="2">
+        <v>5</v>
+      </c>
+      <c r="BG134" s="2">
+        <v>5</v>
+      </c>
+      <c r="BH134" s="2">
+        <v>5</v>
+      </c>
+      <c r="BI134" s="2">
+        <v>4</v>
+      </c>
+      <c r="BJ134" s="2">
+        <v>3</v>
+      </c>
+      <c r="BK134" s="2">
+        <v>6</v>
+      </c>
+      <c r="BL134" s="2">
+        <v>2</v>
+      </c>
+      <c r="BM134" s="2">
+        <v>2</v>
+      </c>
+      <c r="BN134" s="2">
+        <v>4</v>
+      </c>
+      <c r="BO134" s="2">
+        <v>3</v>
+      </c>
+      <c r="BP134" s="2">
+        <v>3</v>
+      </c>
+      <c r="BQ134" s="2">
+        <v>6</v>
+      </c>
+      <c r="BR134" s="2">
+        <v>6</v>
+      </c>
+      <c r="BS134" s="2">
+        <v>6</v>
+      </c>
+      <c r="BT134" s="2">
+        <v>5</v>
+      </c>
+      <c r="BU134" s="2">
+        <v>5</v>
+      </c>
+      <c r="BV134" s="2">
+        <v>5</v>
+      </c>
+      <c r="BW134" s="2">
+        <v>5</v>
+      </c>
+      <c r="BX134" s="2">
+        <v>5</v>
+      </c>
+      <c r="BY134" s="2">
+        <v>4</v>
+      </c>
+      <c r="BZ134" s="3">
+        <v>14.768666666666666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>